<commit_message>
BIS-1050: Fixed failed import when there are inlined images in a property.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_large_cell.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_large_cell.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TYPES" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="99">
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"custom_widget":"Word Processor"}</t>
   </si>
   <si>
     <t xml:space="preserve">EXPERIMENT_TYPE</t>
@@ -327,7 +330,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -378,6 +381,12 @@
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -460,7 +469,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -505,40 +514,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -670,8 +683,8 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -760,7 +773,7 @@
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -773,7 +786,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
@@ -796,7 +809,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>225</v>
       </c>
@@ -813,7 +826,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
@@ -848,7 +861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>225</v>
       </c>
@@ -909,7 +922,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>225</v>
       </c>
@@ -938,7 +951,7 @@
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>225</v>
       </c>
@@ -967,7 +980,7 @@
       <c r="J15" s="10"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>225</v>
       </c>
@@ -996,7 +1009,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <v>225</v>
       </c>
@@ -1025,7 +1038,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
         <v>225</v>
       </c>
@@ -1054,7 +1067,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
         <v>225</v>
       </c>
@@ -1083,7 +1096,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
         <v>225</v>
       </c>
@@ -1112,7 +1125,7 @@
       <c r="J20" s="10"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
         <v>225</v>
       </c>
@@ -1138,7 +1151,9 @@
       <c r="I21" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="J21" s="10"/>
+      <c r="J21" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="K21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1147,11 +1162,11 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="I22" s="11"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1175,7 +1190,7 @@
         <v>225</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="7"/>
@@ -1217,7 +1232,7 @@
         <v>225</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>29</v>
@@ -1226,16 +1241,16 @@
         <v>18</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>46</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,8 +1282,8 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M20" activeCellId="1" sqref="J21 M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1279,7 +1294,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -1293,10 +1308,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,7 +1319,7 @@
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3"/>
     </row>
@@ -1316,18 +1331,18 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,19 +1351,19 @@
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -1357,32 +1372,32 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1392,13 +1407,13 @@
     </row>
     <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -1413,28 +1428,28 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I19" s="17" t="s">
         <v>28</v>
@@ -1457,80 +1472,80 @@
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M20" s="11" t="s">
         <v>92</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="38.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="I22" s="11" t="s">
-        <v>96</v>
+      <c r="I22" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,22 +1553,22 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="19"/>
-      <c r="J23" s="11"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="20"/>
-      <c r="I24" s="11"/>
+      <c r="G24" s="21"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
       <c r="B25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="I25" s="11"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3"/>

</xml_diff>